<commit_message>
SVN Revision #7326 by scriswellwsf       CBECC-22 (1248) executables and ruleset/screens source enabling Community Solar for LowRise Res projects
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24R_CommunitySolar.xlsx
+++ b/RulesetDev/Rulesets/shared/T24R_CommunitySolar.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBAF668-01ED-44F1-A89B-B1BB5EE4D91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7915DA3-B771-4AA9-B6C6-8FFA94AF34FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5528" yWindow="1485" windowWidth="16102" windowHeight="11423" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
+    <workbookView xWindow="285" yWindow="1320" windowWidth="16485" windowHeight="13485" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>kTDV</t>
   </si>
@@ -109,6 +112,18 @@
   </si>
   <si>
     <t>CodeBase</t>
+  </si>
+  <si>
+    <t>SrcKBtu</t>
+  </si>
+  <si>
+    <t>05/25/22 - SAC - added newly calculated SMUD Community Solar results for use in 2022 analysis</t>
+  </si>
+  <si>
+    <t>kBtu of Source Energy (EDR1)</t>
+  </si>
+  <si>
+    <t>06/01/22 - SAC - updated 2022 look-up values w/ latest 2022 kW multipliers</t>
   </si>
 </sst>
 </file>
@@ -194,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +225,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,21 +541,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.3984375" customWidth="1"/>
-    <col min="4" max="4" width="10.53125" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.265625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="8" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -546,7 +563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -554,38 +571,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -596,25 +615,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -622,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -633,7 +655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -644,12 +666,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -658,7 +680,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -669,7 +691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -680,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -691,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -702,95 +724,144 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C23" s="1" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C24" s="8">
+      <c r="I24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="8">
         <v>2019</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="8">
         <v>1</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <v>-2011.8</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>-0.1108</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>-56263</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>-333.12</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C25" s="8" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>-2137.9</v>
+      </c>
+      <c r="F26" s="10">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="G26" s="10">
+        <v>-47454</v>
+      </c>
+      <c r="H26" s="10">
+        <v>-99.150999999999996</v>
+      </c>
+      <c r="I26" s="10">
+        <v>-1609.6</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E27" s="6">
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F27">
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="G27">
         <v>0</v>
       </c>
-      <c r="H25">
+      <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" s="5"/>
-      <c r="B26" t="s">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SVN Revision #7701       CBECC-22 and 2025 (1274) executables, INI files and ruleset source - initial 2025.0.1 research release where 2025 analysis matches 2022
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24R_CommunitySolar.xlsx
+++ b/RulesetDev/Rulesets/shared/T24R_CommunitySolar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7915DA3-B771-4AA9-B6C6-8FFA94AF34FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFAE04E-8AFB-4613-9835-D1BF2BF1F278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="1320" windowWidth="16485" windowHeight="13485" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
+    <workbookView xWindow="2310" yWindow="1830" windowWidth="25800" windowHeight="12645" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>kTDV</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>06/01/22 - SAC - updated 2022 look-up values w/ latest 2022 kW multipliers</t>
+  </si>
+  <si>
+    <t>COPIED from 2022 - MUST BE UPDATED BASED ON 2025 WEATHER &amp; METRICS</t>
+  </si>
+  <si>
+    <t>10/24/22 - SAC - added 2025 code vintage records - copied directly from 2022 values for now - NEEDING UPDATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +165,27 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -209,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +247,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -584,7 +606,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -635,24 +657,22 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,169 +680,151 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="8">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
         <v>2019</v>
-      </c>
-      <c r="D25" s="8">
-        <v>1</v>
-      </c>
-      <c r="E25" s="6">
-        <v>-2011.8</v>
-      </c>
-      <c r="F25">
-        <v>-0.1108</v>
-      </c>
-      <c r="G25">
-        <v>-56263</v>
-      </c>
-      <c r="H25">
-        <v>-333.12</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="8">
-        <v>2022</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="9">
-        <v>-2137.9</v>
-      </c>
-      <c r="F26" s="10">
-        <v>-1.23E-2</v>
-      </c>
-      <c r="G26" s="10">
-        <v>-47454</v>
-      </c>
-      <c r="H26" s="10">
-        <v>-99.150999999999996</v>
-      </c>
-      <c r="I26" s="10">
-        <v>-1609.6</v>
+      <c r="E26" s="6">
+        <v>-2011.8</v>
+      </c>
+      <c r="F26">
+        <v>-0.1108</v>
+      </c>
+      <c r="G26">
+        <v>-56263</v>
+      </c>
+      <c r="H26">
+        <v>-333.12</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>4</v>
@@ -831,37 +833,105 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="8" t="s">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C27" s="8">
+        <v>2022</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>-2137.9</v>
+      </c>
+      <c r="F27" s="10">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="G27" s="10">
+        <v>-47454</v>
+      </c>
+      <c r="H27" s="10">
+        <v>-99.150999999999996</v>
+      </c>
+      <c r="I27" s="10">
+        <v>-1609.6</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C28" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>-2137.9</v>
+      </c>
+      <c r="F28" s="10">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="G28" s="10">
+        <v>-47454</v>
+      </c>
+      <c r="H28" s="10">
+        <v>-99.150999999999996</v>
+      </c>
+      <c r="I28" s="10">
+        <v>-1609.6</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E29" s="6">
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="G29">
         <v>0</v>
       </c>
-      <c r="H27">
+      <c r="H29">
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="I29">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" t="s">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SVN Revision #7701 by scriswellwsf       CBECC-22 and 2025 (1274) executables, INI files and ruleset source - initial 2025.0.1 research release where 2025 analysis matches 2022
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/shared/T24R_CommunitySolar.xlsx
+++ b/RulesetDev/Rulesets/shared/T24R_CommunitySolar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7915DA3-B771-4AA9-B6C6-8FFA94AF34FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFAE04E-8AFB-4613-9835-D1BF2BF1F278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="1320" windowWidth="16485" windowHeight="13485" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
+    <workbookView xWindow="2310" yWindow="1830" windowWidth="25800" windowHeight="12645" xr2:uid="{451AA6B4-8F74-4A09-9E06-84A86EFCFE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>kTDV</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>06/01/22 - SAC - updated 2022 look-up values w/ latest 2022 kW multipliers</t>
+  </si>
+  <si>
+    <t>COPIED from 2022 - MUST BE UPDATED BASED ON 2025 WEATHER &amp; METRICS</t>
+  </si>
+  <si>
+    <t>10/24/22 - SAC - added 2025 code vintage records - copied directly from 2022 values for now - NEEDING UPDATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +165,27 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -209,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +247,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EABD591-F703-4994-B9A0-1B58CC57ECFD}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -584,7 +606,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -635,24 +657,22 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,169 +680,151 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="8">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
         <v>2019</v>
-      </c>
-      <c r="D25" s="8">
-        <v>1</v>
-      </c>
-      <c r="E25" s="6">
-        <v>-2011.8</v>
-      </c>
-      <c r="F25">
-        <v>-0.1108</v>
-      </c>
-      <c r="G25">
-        <v>-56263</v>
-      </c>
-      <c r="H25">
-        <v>-333.12</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="8">
-        <v>2022</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="9">
-        <v>-2137.9</v>
-      </c>
-      <c r="F26" s="10">
-        <v>-1.23E-2</v>
-      </c>
-      <c r="G26" s="10">
-        <v>-47454</v>
-      </c>
-      <c r="H26" s="10">
-        <v>-99.150999999999996</v>
-      </c>
-      <c r="I26" s="10">
-        <v>-1609.6</v>
+      <c r="E26" s="6">
+        <v>-2011.8</v>
+      </c>
+      <c r="F26">
+        <v>-0.1108</v>
+      </c>
+      <c r="G26">
+        <v>-56263</v>
+      </c>
+      <c r="H26">
+        <v>-333.12</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>4</v>
@@ -831,37 +833,105 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="8" t="s">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C27" s="8">
+        <v>2022</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>-2137.9</v>
+      </c>
+      <c r="F27" s="10">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="G27" s="10">
+        <v>-47454</v>
+      </c>
+      <c r="H27" s="10">
+        <v>-99.150999999999996</v>
+      </c>
+      <c r="I27" s="10">
+        <v>-1609.6</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C28" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>-2137.9</v>
+      </c>
+      <c r="F28" s="10">
+        <v>-1.23E-2</v>
+      </c>
+      <c r="G28" s="10">
+        <v>-47454</v>
+      </c>
+      <c r="H28" s="10">
+        <v>-99.150999999999996</v>
+      </c>
+      <c r="I28" s="10">
+        <v>-1609.6</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E29" s="6">
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="G29">
         <v>0</v>
       </c>
-      <c r="H27">
+      <c r="H29">
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="I29">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" t="s">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>